<commit_message>
Atualizando o arquivo XLSX
</commit_message>
<xml_diff>
--- a/jogos_2025-05-01.xlsx
+++ b/jogos_2025-05-01.xlsx
@@ -752,20 +752,20 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>incomplete</t>
+          <t>complete</t>
         </is>
       </c>
       <c r="L2" t="n">
@@ -842,12 +842,12 @@
       </c>
       <c r="AJ2" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['5', '23', '48']</t>
         </is>
       </c>
       <c r="AK2" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['90', '90+7']</t>
         </is>
       </c>
       <c r="AL2" t="n">
@@ -860,7 +860,7 @@
         <v>1.68</v>
       </c>
       <c r="AO2" t="n">
-        <v>-1</v>
+        <v>12</v>
       </c>
       <c r="AP2" t="n">
         <v>1.24</v>
@@ -941,7 +941,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -951,7 +951,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>incomplete</t>
+          <t>complete</t>
         </is>
       </c>
       <c r="L3" t="n">
@@ -1003,16 +1003,16 @@
         <v>10</v>
       </c>
       <c r="AB3" t="n">
-        <v>1.25</v>
+        <v>1.24</v>
       </c>
       <c r="AC3" t="n">
-        <v>3.75</v>
+        <v>3.64</v>
       </c>
       <c r="AD3" t="n">
-        <v>1.61</v>
+        <v>1.57</v>
       </c>
       <c r="AE3" t="n">
-        <v>2.22</v>
+        <v>2.15</v>
       </c>
       <c r="AF3" t="n">
         <v>2.65</v>
@@ -1033,7 +1033,7 @@
       </c>
       <c r="AK3" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['60', '88']</t>
         </is>
       </c>
       <c r="AL3" t="n">
@@ -1046,37 +1046,37 @@
         <v>1.01</v>
       </c>
       <c r="AO3" t="n">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="AP3" t="n">
-        <v>0</v>
+        <v>1.24</v>
       </c>
       <c r="AQ3" t="n">
-        <v>0</v>
+        <v>1.51</v>
       </c>
       <c r="AR3" t="n">
-        <v>0</v>
+        <v>1.84</v>
       </c>
       <c r="AS3" t="n">
-        <v>0</v>
+        <v>2.29</v>
       </c>
       <c r="AT3" t="n">
-        <v>0</v>
+        <v>3.1</v>
       </c>
       <c r="AU3" t="n">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="AV3" t="n">
-        <v>0</v>
+        <v>2.32</v>
       </c>
       <c r="AW3" t="n">
-        <v>0</v>
+        <v>1.82</v>
       </c>
       <c r="AX3" t="n">
-        <v>0</v>
+        <v>1.53</v>
       </c>
       <c r="AY3" t="n">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="AZ3" t="n">
         <v>0</v>
@@ -1124,20 +1124,20 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>incomplete</t>
+          <t>complete</t>
         </is>
       </c>
       <c r="L4" t="n">
@@ -1214,14 +1214,14 @@
       </c>
       <c r="AJ4" t="inlineStr">
         <is>
+          <t>['25', '41']</t>
+        </is>
+      </c>
+      <c r="AK4" t="inlineStr">
+        <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="AK4" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
       <c r="AL4" t="n">
         <v>0</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>0</v>
       </c>
       <c r="AO4" t="n">
-        <v>-1</v>
+        <v>12</v>
       </c>
       <c r="AP4" t="n">
         <v>0</v>
@@ -1310,20 +1310,20 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>incomplete</t>
+          <t>complete</t>
         </is>
       </c>
       <c r="L5" t="n">
@@ -1400,7 +1400,7 @@
       </c>
       <c r="AJ5" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['31']</t>
         </is>
       </c>
       <c r="AK5" t="inlineStr">
@@ -1418,7 +1418,7 @@
         <v>1.36</v>
       </c>
       <c r="AO5" t="n">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="AP5" t="n">
         <v>1.1</v>
@@ -1487,130 +1487,130 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Henan Jianye</t>
+          <t>Zhejiang FC</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Wuhan Three Towns</t>
+          <t>Changchun Yatai</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>incomplete</t>
+          <t>complete</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>1.96</v>
+        <v>1.65</v>
       </c>
       <c r="M6" t="n">
-        <v>3.39</v>
+        <v>3.9</v>
       </c>
       <c r="N6" t="n">
-        <v>3.39</v>
+        <v>4.2</v>
       </c>
       <c r="O6" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="P6" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="R6" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="S6" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="T6" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="U6" t="n">
         <v>1.57</v>
       </c>
-      <c r="P6" t="n">
-        <v>8.5</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="R6" t="n">
-        <v>1.36</v>
-      </c>
-      <c r="S6" t="n">
-        <v>3</v>
-      </c>
-      <c r="T6" t="n">
-        <v>2.63</v>
-      </c>
-      <c r="U6" t="n">
-        <v>1.44</v>
-      </c>
       <c r="V6" t="n">
-        <v>7</v>
+        <v>5.5</v>
       </c>
       <c r="W6" t="n">
-        <v>1.1</v>
+        <v>1.14</v>
       </c>
       <c r="X6" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="Y6" t="n">
-        <v>8.5</v>
+        <v>10</v>
       </c>
       <c r="Z6" t="n">
-        <v>1.25</v>
+        <v>1.17</v>
       </c>
       <c r="AA6" t="n">
-        <v>3.65</v>
+        <v>4.75</v>
       </c>
       <c r="AB6" t="n">
-        <v>1.75</v>
+        <v>1.53</v>
       </c>
       <c r="AC6" t="n">
-        <v>1.91</v>
+        <v>2.25</v>
       </c>
       <c r="AD6" t="n">
-        <v>3</v>
+        <v>2.25</v>
       </c>
       <c r="AE6" t="n">
-        <v>1.36</v>
+        <v>1.57</v>
       </c>
       <c r="AF6" t="n">
-        <v>1.7</v>
+        <v>1.57</v>
       </c>
       <c r="AG6" t="n">
-        <v>2.05</v>
+        <v>2.25</v>
       </c>
       <c r="AH6" t="n">
-        <v>5.15</v>
+        <v>4</v>
       </c>
       <c r="AI6" t="n">
-        <v>1.1</v>
+        <v>1.22</v>
       </c>
       <c r="AJ6" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['9', '24', '45+2', '64']</t>
         </is>
       </c>
       <c r="AK6" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['13', '47']</t>
         </is>
       </c>
       <c r="AL6" t="n">
-        <v>1.28</v>
+        <v>1.15</v>
       </c>
       <c r="AM6" t="n">
-        <v>1.25</v>
+        <v>1.18</v>
       </c>
       <c r="AN6" t="n">
-        <v>1.77</v>
+        <v>2.15</v>
       </c>
       <c r="AO6" t="n">
         <v>-1</v>
       </c>
       <c r="AP6" t="n">
-        <v>1.21</v>
+        <v>1.22</v>
       </c>
       <c r="AQ6" t="n">
-        <v>1.41</v>
+        <v>1.42</v>
       </c>
       <c r="AR6" t="n">
         <v>1.7</v>
@@ -1619,13 +1619,13 @@
         <v>2.05</v>
       </c>
       <c r="AT6" t="n">
-        <v>2.6</v>
+        <v>2.65</v>
       </c>
       <c r="AU6" t="n">
-        <v>3.75</v>
+        <v>3.65</v>
       </c>
       <c r="AV6" t="n">
-        <v>2.7</v>
+        <v>2.65</v>
       </c>
       <c r="AW6" t="n">
         <v>2.05</v>
@@ -1634,19 +1634,19 @@
         <v>1.7</v>
       </c>
       <c r="AY6" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="AZ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB6" t="n">
         <v>1.44</v>
       </c>
-      <c r="AZ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB6" t="n">
-        <v>1.57</v>
-      </c>
       <c r="BC6" t="n">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="BD6" s="3" t="n">
         <v>45778.33333333334</v>
@@ -1673,19 +1673,19 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Zhejiang FC</t>
+          <t>Henan Jianye</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Changchun Yatai</t>
+          <t>Wuhan Three Towns</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -1695,108 +1695,108 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>incomplete</t>
+          <t>complete</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>1.65</v>
+        <v>1.96</v>
       </c>
       <c r="M7" t="n">
-        <v>3.9</v>
+        <v>3.39</v>
       </c>
       <c r="N7" t="n">
-        <v>4.2</v>
+        <v>3.39</v>
       </c>
       <c r="O7" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="P7" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="R7" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="S7" t="n">
+        <v>3</v>
+      </c>
+      <c r="T7" t="n">
+        <v>2.63</v>
+      </c>
+      <c r="U7" t="n">
         <v>1.44</v>
       </c>
-      <c r="P7" t="n">
-        <v>10</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>2.75</v>
-      </c>
-      <c r="R7" t="n">
-        <v>1.29</v>
-      </c>
-      <c r="S7" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="T7" t="n">
-        <v>2.25</v>
-      </c>
-      <c r="U7" t="n">
-        <v>1.57</v>
-      </c>
       <c r="V7" t="n">
-        <v>5.5</v>
+        <v>7</v>
       </c>
       <c r="W7" t="n">
-        <v>1.14</v>
+        <v>1.1</v>
       </c>
       <c r="X7" t="n">
-        <v>1.03</v>
+        <v>1.05</v>
       </c>
       <c r="Y7" t="n">
-        <v>10</v>
+        <v>8.5</v>
       </c>
       <c r="Z7" t="n">
-        <v>1.17</v>
+        <v>1.25</v>
       </c>
       <c r="AA7" t="n">
-        <v>4.75</v>
+        <v>3.65</v>
       </c>
       <c r="AB7" t="n">
-        <v>1.53</v>
+        <v>1.75</v>
       </c>
       <c r="AC7" t="n">
-        <v>2.25</v>
+        <v>1.91</v>
       </c>
       <c r="AD7" t="n">
-        <v>2.25</v>
+        <v>3</v>
       </c>
       <c r="AE7" t="n">
-        <v>1.57</v>
+        <v>1.36</v>
       </c>
       <c r="AF7" t="n">
-        <v>1.57</v>
+        <v>1.7</v>
       </c>
       <c r="AG7" t="n">
-        <v>2.25</v>
+        <v>2.05</v>
       </c>
       <c r="AH7" t="n">
-        <v>4</v>
+        <v>5.15</v>
       </c>
       <c r="AI7" t="n">
-        <v>1.22</v>
+        <v>1.1</v>
       </c>
       <c r="AJ7" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['54']</t>
         </is>
       </c>
       <c r="AK7" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['63', '89']</t>
         </is>
       </c>
       <c r="AL7" t="n">
-        <v>1.15</v>
+        <v>1.28</v>
       </c>
       <c r="AM7" t="n">
-        <v>1.18</v>
+        <v>1.25</v>
       </c>
       <c r="AN7" t="n">
-        <v>2.15</v>
+        <v>1.77</v>
       </c>
       <c r="AO7" t="n">
-        <v>-1</v>
+        <v>11</v>
       </c>
       <c r="AP7" t="n">
-        <v>1.22</v>
+        <v>1.21</v>
       </c>
       <c r="AQ7" t="n">
-        <v>1.42</v>
+        <v>1.41</v>
       </c>
       <c r="AR7" t="n">
         <v>1.7</v>
@@ -1805,13 +1805,13 @@
         <v>2.05</v>
       </c>
       <c r="AT7" t="n">
-        <v>2.65</v>
+        <v>2.6</v>
       </c>
       <c r="AU7" t="n">
-        <v>3.65</v>
+        <v>3.75</v>
       </c>
       <c r="AV7" t="n">
-        <v>2.65</v>
+        <v>2.7</v>
       </c>
       <c r="AW7" t="n">
         <v>2.05</v>
@@ -1820,7 +1820,7 @@
         <v>1.7</v>
       </c>
       <c r="AY7" t="n">
-        <v>1.42</v>
+        <v>1.44</v>
       </c>
       <c r="AZ7" t="n">
         <v>0</v>
@@ -1829,10 +1829,10 @@
         <v>0</v>
       </c>
       <c r="BB7" t="n">
-        <v>1.44</v>
+        <v>1.57</v>
       </c>
       <c r="BC7" t="n">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="BD7" s="3" t="n">
         <v>45778.33333333334</v>
@@ -1868,10 +1868,10 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>incomplete</t>
+          <t>complete</t>
         </is>
       </c>
       <c r="L8" t="n">
@@ -1958,12 +1958,12 @@
       </c>
       <c r="AJ8" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['88']</t>
         </is>
       </c>
       <c r="AK8" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['55', '69', '86']</t>
         </is>
       </c>
       <c r="AL8" t="n">
@@ -1976,7 +1976,7 @@
         <v>1.44</v>
       </c>
       <c r="AO8" t="n">
-        <v>-1</v>
+        <v>11</v>
       </c>
       <c r="AP8" t="n">
         <v>1.24</v>
@@ -2054,20 +2054,20 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>incomplete</t>
+          <t>complete</t>
         </is>
       </c>
       <c r="L9" t="n">
@@ -2144,12 +2144,12 @@
       </c>
       <c r="AJ9" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['40']</t>
         </is>
       </c>
       <c r="AK9" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['42', '55']</t>
         </is>
       </c>
       <c r="AL9" t="n">
@@ -2162,7 +2162,7 @@
         <v>1.67</v>
       </c>
       <c r="AO9" t="n">
-        <v>-1</v>
+        <v>11</v>
       </c>
       <c r="AP9" t="n">
         <v>1.2</v>
@@ -2240,10 +2240,10 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
@@ -2253,7 +2253,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>incomplete</t>
+          <t>complete</t>
         </is>
       </c>
       <c r="L10" t="n">
@@ -2330,12 +2330,12 @@
       </c>
       <c r="AJ10" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['74']</t>
         </is>
       </c>
       <c r="AK10" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['61']</t>
         </is>
       </c>
       <c r="AL10" t="n">
@@ -2348,7 +2348,7 @@
         <v>3.9</v>
       </c>
       <c r="AO10" t="n">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="AP10" t="n">
         <v>1.16</v>
@@ -2426,20 +2426,20 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>incomplete</t>
+          <t>complete</t>
         </is>
       </c>
       <c r="L11" t="n">
@@ -2455,28 +2455,28 @@
         <v>1.44</v>
       </c>
       <c r="P11" t="n">
-        <v>0</v>
+        <v>15.75</v>
       </c>
       <c r="Q11" t="n">
         <v>2.75</v>
       </c>
       <c r="R11" t="n">
-        <v>0</v>
+        <v>1.27</v>
       </c>
       <c r="S11" t="n">
-        <v>0</v>
+        <v>3.28</v>
       </c>
       <c r="T11" t="n">
-        <v>0</v>
+        <v>2.35</v>
       </c>
       <c r="U11" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="V11" t="n">
-        <v>0</v>
+        <v>5.35</v>
       </c>
       <c r="W11" t="n">
-        <v>0</v>
+        <v>1.09</v>
       </c>
       <c r="X11" t="n">
         <v>0</v>
@@ -2485,10 +2485,10 @@
         <v>0</v>
       </c>
       <c r="Z11" t="n">
-        <v>0</v>
+        <v>1.15</v>
       </c>
       <c r="AA11" t="n">
-        <v>0</v>
+        <v>4.25</v>
       </c>
       <c r="AB11" t="n">
         <v>1.6</v>
@@ -2503,68 +2503,68 @@
         <v>1.5</v>
       </c>
       <c r="AF11" t="n">
-        <v>0</v>
+        <v>1.53</v>
       </c>
       <c r="AG11" t="n">
-        <v>0</v>
+        <v>2.28</v>
       </c>
       <c r="AH11" t="n">
-        <v>0</v>
+        <v>4.4</v>
       </c>
       <c r="AI11" t="n">
-        <v>0</v>
+        <v>1.14</v>
       </c>
       <c r="AJ11" t="inlineStr">
         <is>
+          <t>['22', '51', '66', '90+2']</t>
+        </is>
+      </c>
+      <c r="AK11" t="inlineStr">
+        <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="AK11" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
       <c r="AL11" t="n">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="AM11" t="n">
-        <v>0</v>
+        <v>1.21</v>
       </c>
       <c r="AN11" t="n">
-        <v>0</v>
+        <v>1.72</v>
       </c>
       <c r="AO11" t="n">
-        <v>-1</v>
+        <v>22</v>
       </c>
       <c r="AP11" t="n">
         <v>0</v>
       </c>
       <c r="AQ11" t="n">
-        <v>0</v>
+        <v>1.22</v>
       </c>
       <c r="AR11" t="n">
-        <v>0</v>
+        <v>1.41</v>
       </c>
       <c r="AS11" t="n">
-        <v>0</v>
+        <v>1.71</v>
       </c>
       <c r="AT11" t="n">
-        <v>0</v>
+        <v>2.12</v>
       </c>
       <c r="AU11" t="n">
         <v>0</v>
       </c>
       <c r="AV11" t="n">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="AW11" t="n">
-        <v>0</v>
+        <v>2.52</v>
       </c>
       <c r="AX11" t="n">
-        <v>0</v>
+        <v>1.97</v>
       </c>
       <c r="AY11" t="n">
-        <v>0</v>
+        <v>1.58</v>
       </c>
       <c r="AZ11" t="n">
         <v>0</v>
@@ -2680,7 +2680,7 @@
         <v>2</v>
       </c>
       <c r="AC12" t="n">
-        <v>1.67</v>
+        <v>1.75</v>
       </c>
       <c r="AD12" t="n">
         <v>0</v>
@@ -2789,12 +2789,12 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Cosenza</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Bari 1908</t>
+          <t>Südtirol</t>
         </is>
       </c>
       <c r="G13" t="n">
@@ -2815,22 +2815,22 @@
         </is>
       </c>
       <c r="L13" t="n">
-        <v>3.18</v>
+        <v>1.88</v>
       </c>
       <c r="M13" t="n">
-        <v>3.32</v>
+        <v>3.57</v>
       </c>
       <c r="N13" t="n">
-        <v>2.39</v>
+        <v>4.5</v>
       </c>
       <c r="O13" t="n">
-        <v>2.3</v>
+        <v>1.57</v>
       </c>
       <c r="P13" t="n">
         <v>0</v>
       </c>
       <c r="Q13" t="n">
-        <v>1.8</v>
+        <v>2.75</v>
       </c>
       <c r="R13" t="n">
         <v>1.44</v>
@@ -2863,10 +2863,10 @@
         <v>0</v>
       </c>
       <c r="AB13" t="n">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="AC13" t="n">
-        <v>1.6</v>
+        <v>1.82</v>
       </c>
       <c r="AD13" t="n">
         <v>0</v>
@@ -2875,10 +2875,10 @@
         <v>0</v>
       </c>
       <c r="AF13" t="n">
-        <v>1.91</v>
+        <v>1.95</v>
       </c>
       <c r="AG13" t="n">
-        <v>1.91</v>
+        <v>1.8</v>
       </c>
       <c r="AH13" t="n">
         <v>0</v>
@@ -2945,10 +2945,10 @@
         <v>0</v>
       </c>
       <c r="BB13" t="n">
-        <v>2.3</v>
+        <v>1.57</v>
       </c>
       <c r="BC13" t="n">
-        <v>1.8</v>
+        <v>2.75</v>
       </c>
       <c r="BD13" s="3" t="n">
         <v>45778.41666666666</v>
@@ -3161,12 +3161,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Spezia</t>
+          <t>Mantova</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Salernitana</t>
+          <t>Cesena</t>
         </is>
       </c>
       <c r="G15" t="n">
@@ -3187,22 +3187,22 @@
         </is>
       </c>
       <c r="L15" t="n">
-        <v>1.67</v>
+        <v>2.65</v>
       </c>
       <c r="M15" t="n">
-        <v>4</v>
+        <v>3.19</v>
       </c>
       <c r="N15" t="n">
-        <v>5.4</v>
+        <v>2.9</v>
       </c>
       <c r="O15" t="n">
-        <v>1.44</v>
+        <v>1.83</v>
       </c>
       <c r="P15" t="n">
         <v>0</v>
       </c>
       <c r="Q15" t="n">
-        <v>3.1</v>
+        <v>2.1</v>
       </c>
       <c r="R15" t="n">
         <v>1.36</v>
@@ -3217,10 +3217,10 @@
         <v>1.4</v>
       </c>
       <c r="V15" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="W15" t="n">
-        <v>1.1</v>
+        <v>1.08</v>
       </c>
       <c r="X15" t="n">
         <v>0</v>
@@ -3235,10 +3235,10 @@
         <v>0</v>
       </c>
       <c r="AB15" t="n">
-        <v>1.92</v>
+        <v>1.93</v>
       </c>
       <c r="AC15" t="n">
-        <v>1.89</v>
+        <v>1.88</v>
       </c>
       <c r="AD15" t="n">
         <v>0</v>
@@ -3247,10 +3247,10 @@
         <v>0</v>
       </c>
       <c r="AF15" t="n">
-        <v>1.91</v>
+        <v>1.7</v>
       </c>
       <c r="AG15" t="n">
-        <v>1.91</v>
+        <v>2.05</v>
       </c>
       <c r="AH15" t="n">
         <v>0</v>
@@ -3317,10 +3317,10 @@
         <v>0</v>
       </c>
       <c r="BB15" t="n">
-        <v>1.44</v>
+        <v>1.83</v>
       </c>
       <c r="BC15" t="n">
-        <v>3.1</v>
+        <v>2.1</v>
       </c>
       <c r="BD15" s="3" t="n">
         <v>45778.41666666666</v>
@@ -3347,12 +3347,12 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Sampdoria</t>
+          <t>Cosenza</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Cremonese</t>
+          <t>Bari 1908</t>
         </is>
       </c>
       <c r="G16" t="n">
@@ -3373,13 +3373,13 @@
         </is>
       </c>
       <c r="L16" t="n">
-        <v>3.13</v>
+        <v>3.18</v>
       </c>
       <c r="M16" t="n">
-        <v>3.29</v>
+        <v>3.32</v>
       </c>
       <c r="N16" t="n">
-        <v>2.43</v>
+        <v>2.39</v>
       </c>
       <c r="O16" t="n">
         <v>2.3</v>
@@ -3391,16 +3391,16 @@
         <v>1.8</v>
       </c>
       <c r="R16" t="n">
-        <v>1.4</v>
+        <v>1.44</v>
       </c>
       <c r="S16" t="n">
-        <v>2.75</v>
+        <v>2.63</v>
       </c>
       <c r="T16" t="n">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U16" t="n">
-        <v>1.36</v>
+        <v>1.33</v>
       </c>
       <c r="V16" t="n">
         <v>9</v>
@@ -3421,10 +3421,10 @@
         <v>0</v>
       </c>
       <c r="AB16" t="n">
-        <v>1.98</v>
+        <v>2.1</v>
       </c>
       <c r="AC16" t="n">
-        <v>1.77</v>
+        <v>1.6</v>
       </c>
       <c r="AD16" t="n">
         <v>0</v>
@@ -3433,10 +3433,10 @@
         <v>0</v>
       </c>
       <c r="AF16" t="n">
-        <v>1.8</v>
+        <v>1.91</v>
       </c>
       <c r="AG16" t="n">
-        <v>1.95</v>
+        <v>1.91</v>
       </c>
       <c r="AH16" t="n">
         <v>0</v>
@@ -3533,12 +3533,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Sampdoria</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Südtirol</t>
+          <t>Cremonese</t>
         </is>
       </c>
       <c r="G17" t="n">
@@ -3559,34 +3559,34 @@
         </is>
       </c>
       <c r="L17" t="n">
-        <v>1.88</v>
+        <v>3.13</v>
       </c>
       <c r="M17" t="n">
-        <v>3.57</v>
+        <v>3.29</v>
       </c>
       <c r="N17" t="n">
-        <v>4.5</v>
+        <v>2.43</v>
       </c>
       <c r="O17" t="n">
-        <v>1.57</v>
+        <v>2.3</v>
       </c>
       <c r="P17" t="n">
         <v>0</v>
       </c>
       <c r="Q17" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="R17" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="S17" t="n">
         <v>2.75</v>
       </c>
-      <c r="R17" t="n">
-        <v>1.44</v>
-      </c>
-      <c r="S17" t="n">
-        <v>2.63</v>
-      </c>
       <c r="T17" t="n">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U17" t="n">
-        <v>1.33</v>
+        <v>1.36</v>
       </c>
       <c r="V17" t="n">
         <v>9</v>
@@ -3607,10 +3607,10 @@
         <v>0</v>
       </c>
       <c r="AB17" t="n">
-        <v>2</v>
+        <v>1.98</v>
       </c>
       <c r="AC17" t="n">
-        <v>1.82</v>
+        <v>1.77</v>
       </c>
       <c r="AD17" t="n">
         <v>0</v>
@@ -3619,10 +3619,10 @@
         <v>0</v>
       </c>
       <c r="AF17" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="AG17" t="n">
         <v>1.95</v>
-      </c>
-      <c r="AG17" t="n">
-        <v>1.8</v>
       </c>
       <c r="AH17" t="n">
         <v>0</v>
@@ -3689,10 +3689,10 @@
         <v>0</v>
       </c>
       <c r="BB17" t="n">
-        <v>1.57</v>
+        <v>2.3</v>
       </c>
       <c r="BC17" t="n">
-        <v>2.75</v>
+        <v>1.8</v>
       </c>
       <c r="BD17" s="3" t="n">
         <v>45778.41666666666</v>
@@ -3719,12 +3719,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Mantova</t>
+          <t>Spezia</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Cesena</t>
+          <t>Salernitana</t>
         </is>
       </c>
       <c r="G18" t="n">
@@ -3745,22 +3745,22 @@
         </is>
       </c>
       <c r="L18" t="n">
-        <v>2.65</v>
+        <v>1.67</v>
       </c>
       <c r="M18" t="n">
-        <v>3.19</v>
+        <v>4</v>
       </c>
       <c r="N18" t="n">
-        <v>2.9</v>
+        <v>5.4</v>
       </c>
       <c r="O18" t="n">
-        <v>1.83</v>
+        <v>1.44</v>
       </c>
       <c r="P18" t="n">
         <v>0</v>
       </c>
       <c r="Q18" t="n">
-        <v>2.1</v>
+        <v>3.1</v>
       </c>
       <c r="R18" t="n">
         <v>1.36</v>
@@ -3775,10 +3775,10 @@
         <v>1.4</v>
       </c>
       <c r="V18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="W18" t="n">
-        <v>1.08</v>
+        <v>1.1</v>
       </c>
       <c r="X18" t="n">
         <v>0</v>
@@ -3793,10 +3793,10 @@
         <v>0</v>
       </c>
       <c r="AB18" t="n">
-        <v>1.93</v>
+        <v>1.92</v>
       </c>
       <c r="AC18" t="n">
-        <v>1.88</v>
+        <v>1.89</v>
       </c>
       <c r="AD18" t="n">
         <v>0</v>
@@ -3805,10 +3805,10 @@
         <v>0</v>
       </c>
       <c r="AF18" t="n">
-        <v>1.7</v>
+        <v>1.91</v>
       </c>
       <c r="AG18" t="n">
-        <v>2.05</v>
+        <v>1.91</v>
       </c>
       <c r="AH18" t="n">
         <v>0</v>
@@ -3875,10 +3875,10 @@
         <v>0</v>
       </c>
       <c r="BB18" t="n">
-        <v>1.83</v>
+        <v>1.44</v>
       </c>
       <c r="BC18" t="n">
-        <v>2.1</v>
+        <v>3.1</v>
       </c>
       <c r="BD18" s="3" t="n">
         <v>45778.41666666666</v>
@@ -3949,28 +3949,28 @@
         <v>2.5</v>
       </c>
       <c r="R19" t="n">
-        <v>1.42</v>
+        <v>1.43</v>
       </c>
       <c r="S19" t="n">
-        <v>2.55</v>
+        <v>2.6</v>
       </c>
       <c r="T19" t="n">
-        <v>3.2</v>
+        <v>2.87</v>
       </c>
       <c r="U19" t="n">
-        <v>1.28</v>
+        <v>1.36</v>
       </c>
       <c r="V19" t="n">
-        <v>9.5</v>
+        <v>8</v>
       </c>
       <c r="W19" t="n">
-        <v>1</v>
+        <v>1.07</v>
       </c>
       <c r="X19" t="n">
         <v>1.06</v>
       </c>
       <c r="Y19" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Z19" t="n">
         <v>1.4</v>
@@ -3979,28 +3979,28 @@
         <v>2.7</v>
       </c>
       <c r="AB19" t="n">
-        <v>2.2</v>
+        <v>1.93</v>
       </c>
       <c r="AC19" t="n">
-        <v>1.55</v>
+        <v>1.77</v>
       </c>
       <c r="AD19" t="n">
-        <v>4.2</v>
+        <v>3.55</v>
       </c>
       <c r="AE19" t="n">
-        <v>1.18</v>
+        <v>1.24</v>
       </c>
       <c r="AF19" t="n">
-        <v>1.95</v>
+        <v>1.75</v>
       </c>
       <c r="AG19" t="n">
-        <v>1.8</v>
+        <v>1.93</v>
       </c>
       <c r="AH19" t="n">
-        <v>8.5</v>
+        <v>7</v>
       </c>
       <c r="AI19" t="n">
-        <v>1.01</v>
+        <v>1.06</v>
       </c>
       <c r="AJ19" t="inlineStr">
         <is>
@@ -4013,46 +4013,46 @@
         </is>
       </c>
       <c r="AL19" t="n">
-        <v>1.38</v>
+        <v>1.31</v>
       </c>
       <c r="AM19" t="n">
         <v>1.33</v>
       </c>
       <c r="AN19" t="n">
-        <v>1.6</v>
+        <v>1.53</v>
       </c>
       <c r="AO19" t="n">
         <v>-1</v>
       </c>
       <c r="AP19" t="n">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="AQ19" t="n">
-        <v>0</v>
+        <v>1.52</v>
       </c>
       <c r="AR19" t="n">
-        <v>0</v>
+        <v>2.01</v>
       </c>
       <c r="AS19" t="n">
-        <v>0</v>
+        <v>2.24</v>
       </c>
       <c r="AT19" t="n">
-        <v>0</v>
+        <v>2.83</v>
       </c>
       <c r="AU19" t="n">
-        <v>0</v>
+        <v>3.84</v>
       </c>
       <c r="AV19" t="n">
-        <v>0</v>
+        <v>2.48</v>
       </c>
       <c r="AW19" t="n">
-        <v>0</v>
+        <v>1.96</v>
       </c>
       <c r="AX19" t="n">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="AY19" t="n">
-        <v>0</v>
+        <v>1.37</v>
       </c>
       <c r="AZ19" t="n">
         <v>0</v>
@@ -4165,10 +4165,10 @@
         <v>5.75</v>
       </c>
       <c r="AB20" t="n">
-        <v>1.42</v>
+        <v>1.45</v>
       </c>
       <c r="AC20" t="n">
-        <v>2.74</v>
+        <v>2.55</v>
       </c>
       <c r="AD20" t="n">
         <v>1.95</v>
@@ -4303,76 +4303,76 @@
         </is>
       </c>
       <c r="L21" t="n">
-        <v>2.99</v>
+        <v>3.1</v>
       </c>
       <c r="M21" t="n">
-        <v>2.95</v>
+        <v>3</v>
       </c>
       <c r="N21" t="n">
-        <v>2.35</v>
+        <v>2.3</v>
       </c>
       <c r="O21" t="n">
         <v>2.38</v>
       </c>
       <c r="P21" t="n">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="Q21" t="n">
         <v>1.8</v>
       </c>
       <c r="R21" t="n">
-        <v>0</v>
+        <v>1.42</v>
       </c>
       <c r="S21" t="n">
-        <v>0</v>
+        <v>2.52</v>
       </c>
       <c r="T21" t="n">
-        <v>0</v>
+        <v>3.1</v>
       </c>
       <c r="U21" t="n">
-        <v>0</v>
+        <v>1.29</v>
       </c>
       <c r="V21" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W21" t="n">
-        <v>0</v>
+        <v>1.05</v>
       </c>
       <c r="X21" t="n">
-        <v>0</v>
+        <v>1.06</v>
       </c>
       <c r="Y21" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Z21" t="n">
-        <v>0</v>
+        <v>1.37</v>
       </c>
       <c r="AA21" t="n">
-        <v>0</v>
+        <v>2.8</v>
       </c>
       <c r="AB21" t="n">
-        <v>2.25</v>
+        <v>2.1</v>
       </c>
       <c r="AC21" t="n">
-        <v>1.62</v>
+        <v>1.61</v>
       </c>
       <c r="AD21" t="n">
-        <v>0</v>
+        <v>3.9</v>
       </c>
       <c r="AE21" t="n">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="AF21" t="n">
-        <v>0</v>
+        <v>1.85</v>
       </c>
       <c r="AG21" t="n">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="AH21" t="n">
-        <v>0</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="AI21" t="n">
-        <v>0</v>
+        <v>1.02</v>
       </c>
       <c r="AJ21" t="inlineStr">
         <is>
@@ -4385,13 +4385,13 @@
         </is>
       </c>
       <c r="AL21" t="n">
-        <v>0</v>
+        <v>1.28</v>
       </c>
       <c r="AM21" t="n">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="AN21" t="n">
-        <v>0</v>
+        <v>1.68</v>
       </c>
       <c r="AO21" t="n">
         <v>-1</v>
@@ -4835,12 +4835,12 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Chadormalu SC</t>
+          <t>Mes Rafsanjan</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Foolad</t>
+          <t>Persepolis</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -4861,58 +4861,58 @@
         </is>
       </c>
       <c r="L24" t="n">
-        <v>3.3</v>
+        <v>5.5</v>
       </c>
       <c r="M24" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="N24" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0</v>
+      </c>
+      <c r="S24" t="n">
+        <v>0</v>
+      </c>
+      <c r="T24" t="n">
+        <v>0</v>
+      </c>
+      <c r="U24" t="n">
+        <v>0</v>
+      </c>
+      <c r="V24" t="n">
+        <v>0</v>
+      </c>
+      <c r="W24" t="n">
+        <v>0</v>
+      </c>
+      <c r="X24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="AA24" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="AB24" t="n">
         <v>2.55</v>
       </c>
-      <c r="N24" t="n">
-        <v>2.35</v>
-      </c>
-      <c r="O24" t="n">
-        <v>0</v>
-      </c>
-      <c r="P24" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q24" t="n">
-        <v>0</v>
-      </c>
-      <c r="R24" t="n">
-        <v>0</v>
-      </c>
-      <c r="S24" t="n">
-        <v>0</v>
-      </c>
-      <c r="T24" t="n">
-        <v>0</v>
-      </c>
-      <c r="U24" t="n">
-        <v>0</v>
-      </c>
-      <c r="V24" t="n">
-        <v>0</v>
-      </c>
-      <c r="W24" t="n">
-        <v>0</v>
-      </c>
-      <c r="X24" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y24" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB24" t="n">
-        <v>3.3</v>
-      </c>
       <c r="AC24" t="n">
-        <v>1.28</v>
+        <v>1.45</v>
       </c>
       <c r="AD24" t="n">
         <v>0</v>
@@ -5021,12 +5021,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Mes Rafsanjan</t>
+          <t>Chadormalu SC</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Persepolis</t>
+          <t>Foolad</t>
         </is>
       </c>
       <c r="G25" t="n">
@@ -5047,13 +5047,13 @@
         </is>
       </c>
       <c r="L25" t="n">
-        <v>5.5</v>
+        <v>3.3</v>
       </c>
       <c r="M25" t="n">
-        <v>3.5</v>
+        <v>2.55</v>
       </c>
       <c r="N25" t="n">
-        <v>1.53</v>
+        <v>2.35</v>
       </c>
       <c r="O25" t="n">
         <v>0</v>
@@ -5095,10 +5095,10 @@
         <v>0</v>
       </c>
       <c r="AB25" t="n">
-        <v>2.55</v>
+        <v>3.3</v>
       </c>
       <c r="AC25" t="n">
-        <v>1.45</v>
+        <v>1.28</v>
       </c>
       <c r="AD25" t="n">
         <v>0</v>
@@ -5383,7 +5383,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Iran Persian Gulf Pro League</t>
+          <t>Saudi Arabia Professional League</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -5393,12 +5393,12 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Esteghlal Khuzestan</t>
+          <t>Al Riyadh</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Kheybar Khorramabad</t>
+          <t>Al Orubah</t>
         </is>
       </c>
       <c r="G27" t="n">
@@ -5419,76 +5419,76 @@
         </is>
       </c>
       <c r="L27" t="n">
-        <v>2.5</v>
+        <v>1.89</v>
       </c>
       <c r="M27" t="n">
-        <v>2.4</v>
+        <v>3.59</v>
       </c>
       <c r="N27" t="n">
-        <v>3.3</v>
+        <v>3.83</v>
       </c>
       <c r="O27" t="n">
-        <v>2</v>
+        <v>1.53</v>
       </c>
       <c r="P27" t="n">
-        <v>4.33</v>
+        <v>0</v>
       </c>
       <c r="Q27" t="n">
-        <v>2.63</v>
+        <v>2.75</v>
       </c>
       <c r="R27" t="n">
-        <v>1.67</v>
+        <v>1.36</v>
       </c>
       <c r="S27" t="n">
-        <v>2.1</v>
+        <v>3</v>
       </c>
       <c r="T27" t="n">
-        <v>4.5</v>
+        <v>2.75</v>
       </c>
       <c r="U27" t="n">
-        <v>1.2</v>
+        <v>1.4</v>
       </c>
       <c r="V27" t="n">
-        <v>11</v>
+        <v>6.5</v>
       </c>
       <c r="W27" t="n">
-        <v>1.01</v>
+        <v>1.1</v>
       </c>
       <c r="X27" t="n">
-        <v>1.08</v>
+        <v>0</v>
       </c>
       <c r="Y27" t="n">
-        <v>5.45</v>
+        <v>0</v>
       </c>
       <c r="Z27" t="n">
-        <v>1.7</v>
+        <v>0</v>
       </c>
       <c r="AA27" t="n">
-        <v>1.95</v>
+        <v>0</v>
       </c>
       <c r="AB27" t="n">
-        <v>3.21</v>
+        <v>1.9</v>
       </c>
       <c r="AC27" t="n">
-        <v>1.3</v>
+        <v>1.88</v>
       </c>
       <c r="AD27" t="n">
-        <v>7.4</v>
+        <v>0</v>
       </c>
       <c r="AE27" t="n">
-        <v>1.03</v>
+        <v>0</v>
       </c>
       <c r="AF27" t="n">
-        <v>2.4</v>
+        <v>1.8</v>
       </c>
       <c r="AG27" t="n">
-        <v>1.5</v>
+        <v>1.91</v>
       </c>
       <c r="AH27" t="n">
-        <v>14.5</v>
+        <v>0</v>
       </c>
       <c r="AI27" t="n">
-        <v>1.02</v>
+        <v>0</v>
       </c>
       <c r="AJ27" t="inlineStr">
         <is>
@@ -5501,13 +5501,13 @@
         </is>
       </c>
       <c r="AL27" t="n">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="AM27" t="n">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="AN27" t="n">
-        <v>1.46</v>
+        <v>0</v>
       </c>
       <c r="AO27" t="n">
         <v>-1</v>
@@ -5549,10 +5549,10 @@
         <v>0</v>
       </c>
       <c r="BB27" t="n">
-        <v>2</v>
+        <v>1.53</v>
       </c>
       <c r="BC27" t="n">
-        <v>2.63</v>
+        <v>2.75</v>
       </c>
       <c r="BD27" s="3" t="n">
         <v>45778.54166666666</v>
@@ -5569,22 +5569,22 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Norway Eliteserien</t>
+          <t>Iran Persian Gulf Pro League</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2025</t>
+          <t>2024/2025</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Rosenborg</t>
+          <t>Esteghlal Khuzestan</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Kristiansund</t>
+          <t>Kheybar Khorramabad</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -5605,77 +5605,77 @@
         </is>
       </c>
       <c r="L28" t="n">
-        <v>1.24</v>
+        <v>2.5</v>
       </c>
       <c r="M28" t="n">
-        <v>6</v>
+        <v>2.4</v>
       </c>
       <c r="N28" t="n">
-        <v>10</v>
+        <v>3.3</v>
       </c>
       <c r="O28" t="n">
-        <v>1.25</v>
+        <v>2</v>
       </c>
       <c r="P28" t="n">
-        <v>15.5</v>
+        <v>4.33</v>
       </c>
       <c r="Q28" t="n">
-        <v>4</v>
+        <v>2.63</v>
       </c>
       <c r="R28" t="n">
-        <v>1.25</v>
+        <v>1.68</v>
       </c>
       <c r="S28" t="n">
-        <v>3.75</v>
+        <v>2.11</v>
       </c>
       <c r="T28" t="n">
-        <v>2.2</v>
+        <v>4.5</v>
       </c>
       <c r="U28" t="n">
-        <v>1.62</v>
+        <v>1.15</v>
       </c>
       <c r="V28" t="n">
-        <v>5</v>
+        <v>13.5</v>
       </c>
       <c r="W28" t="n">
-        <v>1.17</v>
+        <v>1.03</v>
       </c>
       <c r="X28" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="AB28" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="AC28" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="AD28" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="AE28" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="AF28" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="AG28" t="n">
+        <v>1.52</v>
+      </c>
+      <c r="AH28" t="n">
+        <v>11</v>
+      </c>
+      <c r="AI28" t="n">
         <v>1.01</v>
       </c>
-      <c r="Y28" t="n">
-        <v>17</v>
-      </c>
-      <c r="Z28" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="AA28" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="AB28" t="n">
-        <v>1.47</v>
-      </c>
-      <c r="AC28" t="n">
-        <v>2.57</v>
-      </c>
-      <c r="AD28" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="AE28" t="n">
-        <v>1.55</v>
-      </c>
-      <c r="AF28" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="AG28" t="n">
-        <v>1.95</v>
-      </c>
-      <c r="AH28" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="AI28" t="n">
-        <v>1.25</v>
-      </c>
       <c r="AJ28" t="inlineStr">
         <is>
           <t>[]</t>
@@ -5687,46 +5687,46 @@
         </is>
       </c>
       <c r="AL28" t="n">
-        <v>1.06</v>
+        <v>1.31</v>
       </c>
       <c r="AM28" t="n">
-        <v>1.13</v>
+        <v>1.5</v>
       </c>
       <c r="AN28" t="n">
-        <v>3.75</v>
+        <v>1.46</v>
       </c>
       <c r="AO28" t="n">
         <v>-1</v>
       </c>
       <c r="AP28" t="n">
-        <v>1.1</v>
+        <v>0</v>
       </c>
       <c r="AQ28" t="n">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="AR28" t="n">
-        <v>1.47</v>
+        <v>0</v>
       </c>
       <c r="AS28" t="n">
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="AT28" t="n">
-        <v>2.35</v>
+        <v>0</v>
       </c>
       <c r="AU28" t="n">
-        <v>5.05</v>
+        <v>0</v>
       </c>
       <c r="AV28" t="n">
-        <v>3.4</v>
+        <v>0</v>
       </c>
       <c r="AW28" t="n">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="AX28" t="n">
-        <v>1.83</v>
+        <v>0</v>
       </c>
       <c r="AY28" t="n">
-        <v>1.49</v>
+        <v>0</v>
       </c>
       <c r="AZ28" t="n">
         <v>0</v>
@@ -5735,10 +5735,10 @@
         <v>0</v>
       </c>
       <c r="BB28" t="n">
-        <v>1.25</v>
+        <v>2</v>
       </c>
       <c r="BC28" t="n">
-        <v>4</v>
+        <v>2.63</v>
       </c>
       <c r="BD28" s="3" t="n">
         <v>45778.54166666666</v>
@@ -5755,22 +5755,22 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Saudi Arabia Professional League</t>
+          <t>Norway Eliteserien</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2024/2025</t>
+          <t>2025</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Al Riyadh</t>
+          <t>Rosenborg</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Al Orubah</t>
+          <t>Kristiansund</t>
         </is>
       </c>
       <c r="G29" t="n">
@@ -5791,76 +5791,76 @@
         </is>
       </c>
       <c r="L29" t="n">
-        <v>1.89</v>
+        <v>1.24</v>
       </c>
       <c r="M29" t="n">
-        <v>3.59</v>
+        <v>6</v>
       </c>
       <c r="N29" t="n">
-        <v>3.83</v>
+        <v>10</v>
       </c>
       <c r="O29" t="n">
-        <v>1.53</v>
+        <v>1.25</v>
       </c>
       <c r="P29" t="n">
-        <v>0</v>
+        <v>15.5</v>
       </c>
       <c r="Q29" t="n">
-        <v>2.75</v>
+        <v>4</v>
       </c>
       <c r="R29" t="n">
-        <v>1.36</v>
+        <v>1.25</v>
       </c>
       <c r="S29" t="n">
-        <v>3</v>
+        <v>3.75</v>
       </c>
       <c r="T29" t="n">
-        <v>2.75</v>
+        <v>2.2</v>
       </c>
       <c r="U29" t="n">
-        <v>1.4</v>
+        <v>1.62</v>
       </c>
       <c r="V29" t="n">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="W29" t="n">
-        <v>1.1</v>
+        <v>1.17</v>
       </c>
       <c r="X29" t="n">
-        <v>0</v>
+        <v>1.01</v>
       </c>
       <c r="Y29" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="Z29" t="n">
-        <v>0</v>
+        <v>1.14</v>
       </c>
       <c r="AA29" t="n">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="AB29" t="n">
-        <v>1.9</v>
+        <v>1.47</v>
       </c>
       <c r="AC29" t="n">
-        <v>1.88</v>
+        <v>2.57</v>
       </c>
       <c r="AD29" t="n">
-        <v>0</v>
+        <v>2.2</v>
       </c>
       <c r="AE29" t="n">
-        <v>0</v>
+        <v>1.55</v>
       </c>
       <c r="AF29" t="n">
         <v>1.8</v>
       </c>
       <c r="AG29" t="n">
-        <v>1.91</v>
+        <v>1.95</v>
       </c>
       <c r="AH29" t="n">
-        <v>0</v>
+        <v>3.8</v>
       </c>
       <c r="AI29" t="n">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="AJ29" t="inlineStr">
         <is>
@@ -5873,46 +5873,46 @@
         </is>
       </c>
       <c r="AL29" t="n">
-        <v>0</v>
+        <v>1.06</v>
       </c>
       <c r="AM29" t="n">
-        <v>0</v>
+        <v>1.13</v>
       </c>
       <c r="AN29" t="n">
-        <v>0</v>
+        <v>3.75</v>
       </c>
       <c r="AO29" t="n">
         <v>-1</v>
       </c>
       <c r="AP29" t="n">
-        <v>0</v>
+        <v>1.1</v>
       </c>
       <c r="AQ29" t="n">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="AR29" t="n">
-        <v>0</v>
+        <v>1.47</v>
       </c>
       <c r="AS29" t="n">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="AT29" t="n">
-        <v>0</v>
+        <v>2.35</v>
       </c>
       <c r="AU29" t="n">
-        <v>0</v>
+        <v>5.05</v>
       </c>
       <c r="AV29" t="n">
-        <v>0</v>
+        <v>3.4</v>
       </c>
       <c r="AW29" t="n">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="AX29" t="n">
-        <v>0</v>
+        <v>1.83</v>
       </c>
       <c r="AY29" t="n">
-        <v>0</v>
+        <v>1.49</v>
       </c>
       <c r="AZ29" t="n">
         <v>0</v>
@@ -5921,10 +5921,10 @@
         <v>0</v>
       </c>
       <c r="BB29" t="n">
-        <v>1.53</v>
+        <v>1.25</v>
       </c>
       <c r="BC29" t="n">
-        <v>2.75</v>
+        <v>4</v>
       </c>
       <c r="BD29" s="3" t="n">
         <v>45778.54166666666</v>
@@ -6127,22 +6127,22 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Faroe Islands Faroe Islands Premier League</t>
+          <t>Bulgaria First League</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2025</t>
+          <t>2024/2025</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>KÍ</t>
+          <t>Hebar 1918</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>TB</t>
+          <t>Levski Krumovgrad</t>
         </is>
       </c>
       <c r="G31" t="n">
@@ -6163,128 +6163,128 @@
         </is>
       </c>
       <c r="L31" t="n">
-        <v>1.03</v>
+        <v>2.73</v>
       </c>
       <c r="M31" t="n">
-        <v>14</v>
+        <v>2.97</v>
       </c>
       <c r="N31" t="n">
-        <v>61</v>
+        <v>2.73</v>
       </c>
       <c r="O31" t="n">
-        <v>1.07</v>
+        <v>2.25</v>
       </c>
       <c r="P31" t="n">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="Q31" t="n">
-        <v>9</v>
+        <v>1.91</v>
       </c>
       <c r="R31" t="n">
-        <v>1.18</v>
+        <v>1.4</v>
       </c>
       <c r="S31" t="n">
-        <v>3.9</v>
+        <v>2.6</v>
       </c>
       <c r="T31" t="n">
-        <v>1.91</v>
+        <v>3.15</v>
       </c>
       <c r="U31" t="n">
-        <v>1.8</v>
+        <v>1.3</v>
       </c>
       <c r="V31" t="n">
-        <v>3.8</v>
+        <v>8.75</v>
       </c>
       <c r="W31" t="n">
-        <v>1.22</v>
+        <v>1.06</v>
       </c>
       <c r="X31" t="n">
-        <v>1.01</v>
+        <v>1.02</v>
       </c>
       <c r="Y31" t="n">
-        <v>19</v>
+        <v>6.75</v>
       </c>
       <c r="Z31" t="n">
-        <v>1.09</v>
+        <v>1.35</v>
       </c>
       <c r="AA31" t="n">
-        <v>5.75</v>
+        <v>2.75</v>
       </c>
       <c r="AB31" t="n">
-        <v>1.35</v>
+        <v>2.2</v>
       </c>
       <c r="AC31" t="n">
-        <v>2.94</v>
+        <v>1.55</v>
       </c>
       <c r="AD31" t="n">
-        <v>1.91</v>
+        <v>4.2</v>
       </c>
       <c r="AE31" t="n">
-        <v>1.8</v>
+        <v>1.2</v>
       </c>
       <c r="AF31" t="n">
-        <v>3.9</v>
+        <v>1.95</v>
       </c>
       <c r="AG31" t="n">
-        <v>1.2</v>
+        <v>1.86</v>
       </c>
       <c r="AH31" t="n">
-        <v>2.88</v>
+        <v>6.5</v>
       </c>
       <c r="AI31" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="AJ31" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="AK31" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="AL31" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="AM31" t="n">
         <v>1.32</v>
       </c>
-      <c r="AJ31" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="AK31" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="AL31" t="n">
-        <v>1.04</v>
-      </c>
-      <c r="AM31" t="n">
-        <v>0</v>
-      </c>
       <c r="AN31" t="n">
-        <v>8.1</v>
+        <v>1.53</v>
       </c>
       <c r="AO31" t="n">
         <v>-1</v>
       </c>
       <c r="AP31" t="n">
-        <v>0</v>
+        <v>1.42</v>
       </c>
       <c r="AQ31" t="n">
-        <v>0</v>
+        <v>1.73</v>
       </c>
       <c r="AR31" t="n">
-        <v>0</v>
+        <v>2.53</v>
       </c>
       <c r="AS31" t="n">
-        <v>0</v>
+        <v>2.66</v>
       </c>
       <c r="AT31" t="n">
-        <v>0</v>
+        <v>3.75</v>
       </c>
       <c r="AU31" t="n">
-        <v>0</v>
+        <v>2.93</v>
       </c>
       <c r="AV31" t="n">
-        <v>0</v>
+        <v>2.17</v>
       </c>
       <c r="AW31" t="n">
-        <v>0</v>
+        <v>1.67</v>
       </c>
       <c r="AX31" t="n">
-        <v>0</v>
+        <v>1.37</v>
       </c>
       <c r="AY31" t="n">
-        <v>0</v>
+        <v>1.21</v>
       </c>
       <c r="AZ31" t="n">
         <v>0</v>
@@ -6293,10 +6293,10 @@
         <v>0</v>
       </c>
       <c r="BB31" t="n">
-        <v>1.07</v>
+        <v>2.25</v>
       </c>
       <c r="BC31" t="n">
-        <v>9</v>
+        <v>1.91</v>
       </c>
       <c r="BD31" s="3" t="n">
         <v>45778.5625</v>
@@ -6313,22 +6313,22 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Bulgaria First League</t>
+          <t>Faroe Islands Faroe Islands Premier League</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2024/2025</t>
+          <t>2025</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Hebar 1918</t>
+          <t>KÍ</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Levski Krumovgrad</t>
+          <t>TB</t>
         </is>
       </c>
       <c r="G32" t="n">
@@ -6349,128 +6349,128 @@
         </is>
       </c>
       <c r="L32" t="n">
-        <v>2.73</v>
+        <v>1.03</v>
       </c>
       <c r="M32" t="n">
-        <v>2.97</v>
+        <v>14</v>
       </c>
       <c r="N32" t="n">
-        <v>2.73</v>
+        <v>61</v>
       </c>
       <c r="O32" t="n">
-        <v>2.25</v>
+        <v>1.07</v>
       </c>
       <c r="P32" t="n">
-        <v>7.5</v>
+        <v>21</v>
       </c>
       <c r="Q32" t="n">
-        <v>1.91</v>
+        <v>9</v>
       </c>
       <c r="R32" t="n">
-        <v>1.4</v>
+        <v>1.25</v>
       </c>
       <c r="S32" t="n">
-        <v>2.6</v>
+        <v>3.8</v>
       </c>
       <c r="T32" t="n">
-        <v>3.22</v>
+        <v>2.1</v>
       </c>
       <c r="U32" t="n">
-        <v>1.3</v>
+        <v>1.67</v>
       </c>
       <c r="V32" t="n">
-        <v>8.6</v>
+        <v>4.33</v>
       </c>
       <c r="W32" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="X32" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>21</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="AC32" t="n">
+        <v>2.94</v>
+      </c>
+      <c r="AD32" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="AE32" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="AF32" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="AG32" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="AH32" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="AI32" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="AJ32" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="AK32" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="AL32" t="n">
         <v>1.04</v>
       </c>
-      <c r="X32" t="n">
-        <v>1.02</v>
-      </c>
-      <c r="Y32" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="Z32" t="n">
-        <v>1.38</v>
-      </c>
-      <c r="AA32" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="AB32" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="AC32" t="n">
-        <v>1.55</v>
-      </c>
-      <c r="AD32" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="AE32" t="n">
-        <v>1.16</v>
-      </c>
-      <c r="AF32" t="n">
-        <v>1.91</v>
-      </c>
-      <c r="AG32" t="n">
-        <v>1.77</v>
-      </c>
-      <c r="AH32" t="n">
-        <v>8.699999999999999</v>
-      </c>
-      <c r="AI32" t="n">
-        <v>1.05</v>
-      </c>
-      <c r="AJ32" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="AK32" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="AL32" t="n">
-        <v>1.3</v>
-      </c>
       <c r="AM32" t="n">
-        <v>1.32</v>
+        <v>1.04</v>
       </c>
       <c r="AN32" t="n">
-        <v>1.65</v>
+        <v>8.5</v>
       </c>
       <c r="AO32" t="n">
         <v>-1</v>
       </c>
       <c r="AP32" t="n">
-        <v>1.42</v>
+        <v>0</v>
       </c>
       <c r="AQ32" t="n">
-        <v>1.72</v>
+        <v>0</v>
       </c>
       <c r="AR32" t="n">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="AS32" t="n">
-        <v>2.92</v>
+        <v>0</v>
       </c>
       <c r="AT32" t="n">
-        <v>3.55</v>
+        <v>0</v>
       </c>
       <c r="AU32" t="n">
-        <v>2.67</v>
+        <v>0</v>
       </c>
       <c r="AV32" t="n">
-        <v>2.06</v>
+        <v>0</v>
       </c>
       <c r="AW32" t="n">
-        <v>1.64</v>
+        <v>0</v>
       </c>
       <c r="AX32" t="n">
-        <v>1.31</v>
+        <v>0</v>
       </c>
       <c r="AY32" t="n">
-        <v>1.24</v>
+        <v>0</v>
       </c>
       <c r="AZ32" t="n">
         <v>0</v>
@@ -6479,10 +6479,10 @@
         <v>0</v>
       </c>
       <c r="BB32" t="n">
-        <v>2.25</v>
+        <v>1.07</v>
       </c>
       <c r="BC32" t="n">
-        <v>1.91</v>
+        <v>9</v>
       </c>
       <c r="BD32" s="3" t="n">
         <v>45778.5625</v>
@@ -6499,7 +6499,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>UAE Arabian Gulf League</t>
+          <t>Jordan Jordanian Pro League</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -6509,12 +6509,12 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Al Sharjah</t>
+          <t>Aqaba</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Bani Yas</t>
+          <t>Al Jazeera</t>
         </is>
       </c>
       <c r="G33" t="n">
@@ -6535,95 +6535,95 @@
         </is>
       </c>
       <c r="L33" t="n">
-        <v>1.29</v>
+        <v>4.2</v>
       </c>
       <c r="M33" t="n">
-        <v>5.25</v>
+        <v>3.3</v>
       </c>
       <c r="N33" t="n">
-        <v>9</v>
+        <v>1.83</v>
       </c>
       <c r="O33" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="P33" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="R33" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="S33" t="n">
+        <v>2.76</v>
+      </c>
+      <c r="T33" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="U33" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="V33" t="n">
+        <v>6</v>
+      </c>
+      <c r="W33" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="X33" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>3.34</v>
+      </c>
+      <c r="AB33" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="AC33" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="AD33" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="AE33" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="AF33" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="AG33" t="n">
+        <v>1.93</v>
+      </c>
+      <c r="AH33" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="AI33" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="AJ33" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="AK33" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="AL33" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="AM33" t="n">
         <v>1.25</v>
       </c>
-      <c r="P33" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q33" t="n">
-        <v>4</v>
-      </c>
-      <c r="R33" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="S33" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="T33" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="U33" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="V33" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="W33" t="n">
-        <v>1.13</v>
-      </c>
-      <c r="X33" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y33" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB33" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="AC33" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="AD33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF33" t="n">
-        <v>2</v>
-      </c>
-      <c r="AG33" t="n">
-        <v>1.73</v>
-      </c>
-      <c r="AH33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ33" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="AK33" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="AL33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM33" t="n">
-        <v>0</v>
-      </c>
       <c r="AN33" t="n">
-        <v>0</v>
+        <v>1.15</v>
       </c>
       <c r="AO33" t="n">
         <v>-1</v>
@@ -6665,10 +6665,10 @@
         <v>0</v>
       </c>
       <c r="BB33" t="n">
-        <v>1.25</v>
+        <v>2.75</v>
       </c>
       <c r="BC33" t="n">
-        <v>4</v>
+        <v>1.53</v>
       </c>
       <c r="BD33" s="3" t="n">
         <v>45778.57291666666</v>
@@ -6685,7 +6685,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Jordan Jordanian Pro League</t>
+          <t>UAE Arabian Gulf League</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -6695,12 +6695,12 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Aqaba</t>
+          <t>Al Sharjah</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Al Jazeera</t>
+          <t>Bani Yas</t>
         </is>
       </c>
       <c r="G34" t="n">
@@ -6721,40 +6721,40 @@
         </is>
       </c>
       <c r="L34" t="n">
-        <v>4.12</v>
+        <v>1.29</v>
       </c>
       <c r="M34" t="n">
-        <v>3.34</v>
+        <v>5.25</v>
       </c>
       <c r="N34" t="n">
-        <v>1.8</v>
+        <v>9</v>
       </c>
       <c r="O34" t="n">
-        <v>2.75</v>
+        <v>1.25</v>
       </c>
       <c r="P34" t="n">
         <v>0</v>
       </c>
       <c r="Q34" t="n">
-        <v>1.53</v>
+        <v>4</v>
       </c>
       <c r="R34" t="n">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="S34" t="n">
-        <v>0</v>
+        <v>3.4</v>
       </c>
       <c r="T34" t="n">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="U34" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="V34" t="n">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="W34" t="n">
-        <v>0</v>
+        <v>1.13</v>
       </c>
       <c r="X34" t="n">
         <v>0</v>
@@ -6769,10 +6769,10 @@
         <v>0</v>
       </c>
       <c r="AB34" t="n">
-        <v>1.87</v>
+        <v>1.6</v>
       </c>
       <c r="AC34" t="n">
-        <v>1.87</v>
+        <v>2.1</v>
       </c>
       <c r="AD34" t="n">
         <v>0</v>
@@ -6781,10 +6781,10 @@
         <v>0</v>
       </c>
       <c r="AF34" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG34" t="n">
-        <v>0</v>
+        <v>1.73</v>
       </c>
       <c r="AH34" t="n">
         <v>0</v>
@@ -6803,13 +6803,13 @@
         </is>
       </c>
       <c r="AL34" t="n">
-        <v>0</v>
+        <v>1.14</v>
       </c>
       <c r="AM34" t="n">
-        <v>0</v>
+        <v>1.23</v>
       </c>
       <c r="AN34" t="n">
-        <v>0</v>
+        <v>2.43</v>
       </c>
       <c r="AO34" t="n">
         <v>-1</v>
@@ -6818,13 +6818,13 @@
         <v>0</v>
       </c>
       <c r="AQ34" t="n">
-        <v>0</v>
+        <v>1.65</v>
       </c>
       <c r="AR34" t="n">
-        <v>0</v>
+        <v>2.09</v>
       </c>
       <c r="AS34" t="n">
-        <v>0</v>
+        <v>2.53</v>
       </c>
       <c r="AT34" t="n">
         <v>0</v>
@@ -6833,13 +6833,13 @@
         <v>0</v>
       </c>
       <c r="AV34" t="n">
-        <v>0</v>
+        <v>2.11</v>
       </c>
       <c r="AW34" t="n">
-        <v>0</v>
+        <v>1.66</v>
       </c>
       <c r="AX34" t="n">
-        <v>0</v>
+        <v>1.44</v>
       </c>
       <c r="AY34" t="n">
         <v>0</v>
@@ -6851,10 +6851,10 @@
         <v>0</v>
       </c>
       <c r="BB34" t="n">
-        <v>2.75</v>
+        <v>1.25</v>
       </c>
       <c r="BC34" t="n">
-        <v>1.53</v>
+        <v>4</v>
       </c>
       <c r="BD34" s="3" t="n">
         <v>45778.57291666666</v>
@@ -6925,34 +6925,34 @@
         <v>1.9</v>
       </c>
       <c r="R35" t="n">
-        <v>1.44</v>
+        <v>1.55</v>
       </c>
       <c r="S35" t="n">
-        <v>2.49</v>
+        <v>2.25</v>
       </c>
       <c r="T35" t="n">
-        <v>3.55</v>
+        <v>3.7</v>
       </c>
       <c r="U35" t="n">
         <v>1.29</v>
       </c>
       <c r="V35" t="n">
-        <v>8.5</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="W35" t="n">
-        <v>1.03</v>
+        <v>1.05</v>
       </c>
       <c r="X35" t="n">
-        <v>1.06</v>
+        <v>1.1</v>
       </c>
       <c r="Y35" t="n">
-        <v>6.5</v>
+        <v>6.25</v>
       </c>
       <c r="Z35" t="n">
-        <v>1.43</v>
+        <v>1.62</v>
       </c>
       <c r="AA35" t="n">
-        <v>2.5</v>
+        <v>2.18</v>
       </c>
       <c r="AB35" t="n">
         <v>2.3</v>
@@ -6961,22 +6961,22 @@
         <v>1.5</v>
       </c>
       <c r="AD35" t="n">
-        <v>4.75</v>
+        <v>6.34</v>
       </c>
       <c r="AE35" t="n">
-        <v>1.18</v>
+        <v>1.17</v>
       </c>
       <c r="AF35" t="n">
-        <v>2</v>
+        <v>2.3</v>
       </c>
       <c r="AG35" t="n">
-        <v>1.77</v>
+        <v>1.7</v>
       </c>
       <c r="AH35" t="n">
-        <v>8.5</v>
+        <v>10</v>
       </c>
       <c r="AI35" t="n">
-        <v>1.01</v>
+        <v>1.03</v>
       </c>
       <c r="AJ35" t="inlineStr">
         <is>
@@ -6989,46 +6989,46 @@
         </is>
       </c>
       <c r="AL35" t="n">
-        <v>1.57</v>
+        <v>1.37</v>
       </c>
       <c r="AM35" t="n">
         <v>1.35</v>
       </c>
       <c r="AN35" t="n">
-        <v>1.16</v>
+        <v>1.33</v>
       </c>
       <c r="AO35" t="n">
         <v>-1</v>
       </c>
       <c r="AP35" t="n">
-        <v>1.32</v>
+        <v>1.28</v>
       </c>
       <c r="AQ35" t="n">
-        <v>1.57</v>
+        <v>1.65</v>
       </c>
       <c r="AR35" t="n">
-        <v>1.93</v>
+        <v>2.1</v>
       </c>
       <c r="AS35" t="n">
         <v>2.49</v>
       </c>
       <c r="AT35" t="n">
-        <v>3.34</v>
+        <v>3.5</v>
       </c>
       <c r="AU35" t="n">
-        <v>3.1</v>
+        <v>3.05</v>
       </c>
       <c r="AV35" t="n">
-        <v>2.31</v>
+        <v>2.1</v>
       </c>
       <c r="AW35" t="n">
-        <v>1.78</v>
+        <v>1.67</v>
       </c>
       <c r="AX35" t="n">
         <v>1.51</v>
       </c>
       <c r="AY35" t="n">
-        <v>1.24</v>
+        <v>1.22</v>
       </c>
       <c r="AZ35" t="n">
         <v>0</v>
@@ -7669,34 +7669,34 @@
         <v>3.4</v>
       </c>
       <c r="R39" t="n">
-        <v>1.55</v>
+        <v>1.5</v>
       </c>
       <c r="S39" t="n">
-        <v>2.25</v>
+        <v>2.4</v>
       </c>
       <c r="T39" t="n">
-        <v>3.65</v>
+        <v>3.48</v>
       </c>
       <c r="U39" t="n">
-        <v>1.23</v>
+        <v>1.3</v>
       </c>
       <c r="V39" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="W39" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="X39" t="n">
-        <v>1.06</v>
+        <v>1.1</v>
       </c>
       <c r="Y39" t="n">
-        <v>6.1</v>
+        <v>6.25</v>
       </c>
       <c r="Z39" t="n">
-        <v>1.47</v>
+        <v>1.5</v>
       </c>
       <c r="AA39" t="n">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="AB39" t="n">
         <v>2.15</v>
@@ -7705,22 +7705,22 @@
         <v>1.57</v>
       </c>
       <c r="AD39" t="n">
-        <v>4.8</v>
+        <v>4.6</v>
       </c>
       <c r="AE39" t="n">
-        <v>1.12</v>
+        <v>1.13</v>
       </c>
       <c r="AF39" t="n">
-        <v>2.25</v>
+        <v>2</v>
       </c>
       <c r="AG39" t="n">
-        <v>1.57</v>
+        <v>1.62</v>
       </c>
       <c r="AH39" t="n">
-        <v>10</v>
+        <v>8.75</v>
       </c>
       <c r="AI39" t="n">
-        <v>1.02</v>
+        <v>1.06</v>
       </c>
       <c r="AJ39" t="inlineStr">
         <is>
@@ -7733,13 +7733,13 @@
         </is>
       </c>
       <c r="AL39" t="n">
-        <v>1.3</v>
+        <v>1.25</v>
       </c>
       <c r="AM39" t="n">
         <v>1.28</v>
       </c>
       <c r="AN39" t="n">
-        <v>1.94</v>
+        <v>1.78</v>
       </c>
       <c r="AO39" t="n">
         <v>-1</v>
@@ -7837,13 +7837,13 @@
         </is>
       </c>
       <c r="L40" t="n">
-        <v>1.36</v>
+        <v>1.39</v>
       </c>
       <c r="M40" t="n">
-        <v>5.34</v>
+        <v>5</v>
       </c>
       <c r="N40" t="n">
-        <v>6.6</v>
+        <v>5.5</v>
       </c>
       <c r="O40" t="n">
         <v>1.25</v>
@@ -7855,10 +7855,10 @@
         <v>4.33</v>
       </c>
       <c r="R40" t="n">
-        <v>1.25</v>
+        <v>1.27</v>
       </c>
       <c r="S40" t="n">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="T40" t="n">
         <v>2.3</v>
@@ -7870,43 +7870,43 @@
         <v>5</v>
       </c>
       <c r="W40" t="n">
-        <v>1.15</v>
+        <v>1.13</v>
       </c>
       <c r="X40" t="n">
-        <v>1.01</v>
+        <v>1</v>
       </c>
       <c r="Y40" t="n">
-        <v>12.9</v>
+        <v>12</v>
       </c>
       <c r="Z40" t="n">
-        <v>1.14</v>
+        <v>1.19</v>
       </c>
       <c r="AA40" t="n">
         <v>4.33</v>
       </c>
       <c r="AB40" t="n">
-        <v>1.63</v>
+        <v>1.61</v>
       </c>
       <c r="AC40" t="n">
-        <v>2.15</v>
+        <v>2.1</v>
       </c>
       <c r="AD40" t="n">
-        <v>2.62</v>
+        <v>2.49</v>
       </c>
       <c r="AE40" t="n">
-        <v>1.38</v>
+        <v>1.49</v>
       </c>
       <c r="AF40" t="n">
-        <v>1.91</v>
+        <v>1.85</v>
       </c>
       <c r="AG40" t="n">
-        <v>1.74</v>
+        <v>1.82</v>
       </c>
       <c r="AH40" t="n">
-        <v>5</v>
+        <v>4.65</v>
       </c>
       <c r="AI40" t="n">
-        <v>1.1</v>
+        <v>1.2</v>
       </c>
       <c r="AJ40" t="inlineStr">
         <is>
@@ -7919,46 +7919,46 @@
         </is>
       </c>
       <c r="AL40" t="n">
-        <v>1.11</v>
+        <v>1.17</v>
       </c>
       <c r="AM40" t="n">
         <v>0</v>
       </c>
       <c r="AN40" t="n">
-        <v>3</v>
+        <v>2.92</v>
       </c>
       <c r="AO40" t="n">
         <v>-1</v>
       </c>
       <c r="AP40" t="n">
-        <v>1.25</v>
+        <v>1.22</v>
       </c>
       <c r="AQ40" t="n">
         <v>1.43</v>
       </c>
       <c r="AR40" t="n">
-        <v>1.78</v>
+        <v>1.99</v>
       </c>
       <c r="AS40" t="n">
-        <v>2.23</v>
+        <v>2.24</v>
       </c>
       <c r="AT40" t="n">
-        <v>2.8</v>
+        <v>2.97</v>
       </c>
       <c r="AU40" t="n">
-        <v>3.42</v>
+        <v>3.5</v>
       </c>
       <c r="AV40" t="n">
-        <v>2.51</v>
+        <v>2.46</v>
       </c>
       <c r="AW40" t="n">
-        <v>1.97</v>
+        <v>1.9</v>
       </c>
       <c r="AX40" t="n">
-        <v>1.61</v>
+        <v>1.52</v>
       </c>
       <c r="AY40" t="n">
-        <v>1.38</v>
+        <v>1.3</v>
       </c>
       <c r="AZ40" t="n">
         <v>0</v>

</xml_diff>